<commit_message>
updates post week 12
</commit_message>
<xml_diff>
--- a/playoff_projection.xlsx
+++ b/playoff_projection.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brendan\PycharmProjects\FFB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PyCharm\Projects\FFB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -451,20 +451,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="15" width="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +520,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -576,18 +576,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.98599999999999999</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>1.35E-2</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>5.0000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -623,42 +623,42 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>1.0145</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="1">
         <v>1</v>
       </c>
       <c r="R3" s="2">
-        <v>0.99950000000000006</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1.21E-2</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.52210000000000001</v>
+        <v>0.96840000000000004</v>
       </c>
       <c r="D4">
-        <v>0.24279999999999999</v>
+        <v>3.1600000000000003E-2</v>
       </c>
       <c r="E4">
-        <v>0.1125</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>6.2199999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>3.56E-2</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>1.17E-2</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -679,42 +679,42 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>2.8492000000000002</v>
+        <v>2.0316000000000001</v>
       </c>
       <c r="Q4" s="1">
-        <v>0.98729999999999996</v>
+        <v>1</v>
       </c>
       <c r="R4" s="2">
-        <v>0.53420000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.96840000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>1.6999999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0.29870000000000002</v>
+        <v>3.1600000000000003E-2</v>
       </c>
       <c r="D5">
-        <v>0.37240000000000001</v>
+        <v>0.46310000000000001</v>
       </c>
       <c r="E5">
-        <v>0.17269999999999999</v>
+        <v>0.2505</v>
       </c>
       <c r="F5">
-        <v>9.2600000000000002E-2</v>
+        <v>0.20230000000000001</v>
       </c>
       <c r="G5">
-        <v>4.9799999999999997E-2</v>
+        <v>5.1200000000000002E-2</v>
       </c>
       <c r="H5">
-        <v>1.11E-2</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="I5">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -735,354 +735,354 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>3.2545999999999999</v>
+        <v>3.7823000000000002</v>
       </c>
       <c r="Q5" s="1">
-        <v>0.9879</v>
+        <v>0.99870000000000003</v>
       </c>
       <c r="R5" s="2">
-        <v>0.3004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>3.1600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.27029999999999998</v>
+      </c>
+      <c r="F6">
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>7.7399999999999997E-2</v>
+      </c>
+      <c r="H6">
+        <v>0.14269999999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.1154</v>
+      </c>
+      <c r="J6">
+        <v>5.1200000000000002E-2</v>
+      </c>
+      <c r="K6">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>5.1950000000000003</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0.68320000000000003</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.1852</v>
+      </c>
+      <c r="E7">
+        <v>0.15240000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.11990000000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.22389999999999999</v>
+      </c>
+      <c r="H7">
+        <v>0.2036</v>
+      </c>
+      <c r="I7">
+        <v>9.6699999999999994E-2</v>
+      </c>
+      <c r="J7">
+        <v>1.83E-2</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>5.4715999999999996</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0.68140000000000001</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>7.5499999999999998E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.22650000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.21290000000000001</v>
+      </c>
+      <c r="G8">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="H8">
+        <v>0.115</v>
+      </c>
+      <c r="I8">
+        <v>0.1678</v>
+      </c>
+      <c r="J8">
+        <v>9.7299999999999998E-2</v>
+      </c>
+      <c r="K8">
+        <v>1.9E-2</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>5.9260999999999999</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0.60089999999999999</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="E9">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.1532</v>
+      </c>
+      <c r="G9">
+        <v>0.16919999999999999</v>
+      </c>
+      <c r="H9">
+        <v>0.1134</v>
+      </c>
+      <c r="I9">
+        <v>0.19950000000000001</v>
+      </c>
+      <c r="J9">
+        <v>0.22839999999999999</v>
+      </c>
+      <c r="K9">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="L9">
+        <v>1.8E-3</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>7.2933000000000003</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0.37190000000000001</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="C6">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="D6">
-        <v>0.24840000000000001</v>
-      </c>
-      <c r="E6">
-        <v>0.30809999999999998</v>
-      </c>
-      <c r="F6">
-        <v>0.1394</v>
-      </c>
-      <c r="G6">
-        <v>9.3299999999999994E-2</v>
-      </c>
-      <c r="H6">
-        <v>4.82E-2</v>
-      </c>
-      <c r="I6">
-        <v>1.4800000000000001E-2</v>
-      </c>
-      <c r="J6">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>3.9967999999999999</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>0.93540000000000001</v>
-      </c>
-      <c r="R6" s="2">
-        <v>0.1462</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>1.46E-2</v>
-      </c>
-      <c r="D7">
-        <v>6.7599999999999993E-2</v>
-      </c>
-      <c r="E7">
-        <v>0.154</v>
-      </c>
-      <c r="F7">
-        <v>0.22090000000000001</v>
-      </c>
-      <c r="G7">
-        <v>0.19120000000000001</v>
-      </c>
-      <c r="H7">
-        <v>0.1183</v>
-      </c>
-      <c r="I7">
-        <v>0.10920000000000001</v>
-      </c>
-      <c r="J7">
-        <v>8.1299999999999997E-2</v>
-      </c>
-      <c r="K7">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="L7">
-        <v>6.4000000000000003E-3</v>
-      </c>
-      <c r="M7">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="N7">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>1E-4</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>5.9706000000000001</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0.64829999999999999</v>
-      </c>
-      <c r="R7" s="2">
-        <v>1.46E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E10">
+        <v>3.04E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.1192</v>
+      </c>
+      <c r="G10">
+        <v>0.17949999999999999</v>
+      </c>
+      <c r="H10">
+        <v>0.13189999999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.111</v>
+      </c>
+      <c r="J10">
+        <v>0.2145</v>
+      </c>
+      <c r="K10">
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="L10">
+        <v>1.72E-2</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>7.6879</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0.32919999999999999</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="D8">
-        <v>3.1699999999999999E-2</v>
-      </c>
-      <c r="E8">
-        <v>0.1111</v>
-      </c>
-      <c r="F8">
-        <v>0.1774</v>
-      </c>
-      <c r="G8">
-        <v>0.14630000000000001</v>
-      </c>
-      <c r="H8">
-        <v>0.18809999999999999</v>
-      </c>
-      <c r="I8">
-        <v>0.1628</v>
-      </c>
-      <c r="J8">
-        <v>8.5599999999999996E-2</v>
-      </c>
-      <c r="K8">
-        <v>5.8799999999999998E-2</v>
-      </c>
-      <c r="L8">
-        <v>2.9499999999999998E-2</v>
-      </c>
-      <c r="M8">
-        <v>5.7999999999999996E-3</v>
-      </c>
-      <c r="N8">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>6.6894</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>0.46870000000000001</v>
-      </c>
-      <c r="R8" s="2">
-        <v>2.2000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>1.6999999999999999E-3</v>
-      </c>
-      <c r="D9">
-        <v>2.2599999999999999E-2</v>
-      </c>
-      <c r="E9">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="F9">
-        <v>0.1386</v>
-      </c>
-      <c r="G9">
-        <v>0.15540000000000001</v>
-      </c>
-      <c r="H9">
-        <v>0.19650000000000001</v>
-      </c>
-      <c r="I9">
-        <v>0.1673</v>
-      </c>
-      <c r="J9">
-        <v>9.7799999999999998E-2</v>
-      </c>
-      <c r="K9">
-        <v>8.0799999999999997E-2</v>
-      </c>
-      <c r="L9">
-        <v>4.3400000000000001E-2</v>
-      </c>
-      <c r="M9">
-        <v>1.12E-2</v>
-      </c>
-      <c r="N9">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>7.0556000000000001</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>0.40229999999999999</v>
-      </c>
-      <c r="R9" s="2">
-        <v>1.6999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="D10">
-        <v>1.32E-2</v>
-      </c>
-      <c r="E10">
-        <v>4.3900000000000002E-2</v>
-      </c>
-      <c r="F10">
-        <v>9.8699999999999996E-2</v>
-      </c>
-      <c r="G10">
-        <v>0.17019999999999999</v>
-      </c>
-      <c r="H10">
-        <v>0.1812</v>
-      </c>
-      <c r="I10">
-        <v>0.12889999999999999</v>
-      </c>
-      <c r="J10">
-        <v>0.13270000000000001</v>
-      </c>
-      <c r="K10">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="L10">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="M10">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>1.77E-2</v>
       </c>
-      <c r="N10">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>7.6375000000000002</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>0.32719999999999999</v>
-      </c>
-      <c r="R10" s="2">
-        <v>1.1999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="E11">
-        <v>6.1000000000000004E-3</v>
-      </c>
-      <c r="F11">
-        <v>3.4500000000000003E-2</v>
-      </c>
       <c r="G11">
-        <v>7.6600000000000001E-2</v>
+        <v>0.10390000000000001</v>
       </c>
       <c r="H11">
-        <v>8.4400000000000003E-2</v>
+        <v>0.2142</v>
       </c>
       <c r="I11">
-        <v>0.1043</v>
+        <v>0.22170000000000001</v>
       </c>
       <c r="J11">
-        <v>0.15870000000000001</v>
+        <v>0.1119</v>
       </c>
       <c r="K11">
-        <v>0.17460000000000001</v>
+        <v>0.2218</v>
       </c>
       <c r="L11">
-        <v>0.11899999999999999</v>
+        <v>0.1085</v>
       </c>
       <c r="M11">
-        <v>0.11749999999999999</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="N11">
-        <v>0.1042</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <v>1.9699999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>9.6066000000000003</v>
+        <v>8.4070999999999998</v>
       </c>
       <c r="Q11" s="1">
-        <v>0.1176</v>
+        <v>0.1216</v>
       </c>
       <c r="R11" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1094,220 +1094,220 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="E12">
-        <v>7.6E-3</v>
+        <v>2.1499999999999998E-2</v>
       </c>
       <c r="F12">
-        <v>3.5000000000000003E-2</v>
+        <v>8.2299999999999998E-2</v>
       </c>
       <c r="G12">
-        <v>6.7199999999999996E-2</v>
+        <v>0.1089</v>
       </c>
       <c r="H12">
-        <v>7.7799999999999994E-2</v>
+        <v>7.7399999999999997E-2</v>
       </c>
       <c r="I12">
-        <v>0.1171</v>
+        <v>8.3299999999999999E-2</v>
       </c>
       <c r="J12">
-        <v>0.17519999999999999</v>
+        <v>0.24590000000000001</v>
       </c>
       <c r="K12">
-        <v>0.1482</v>
+        <v>0.33750000000000002</v>
       </c>
       <c r="L12">
-        <v>0.12520000000000001</v>
+        <v>4.2799999999999998E-2</v>
       </c>
       <c r="M12">
-        <v>0.13919999999999999</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>8.9599999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="O12">
-        <v>1.7500000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <v>9.6074000000000002</v>
+        <v>8.4192</v>
       </c>
       <c r="Q12" s="1">
-        <v>0.11020000000000001</v>
+        <v>0.21310000000000001</v>
       </c>
       <c r="R12" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I13">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="J13">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="K13">
+        <v>0.13270000000000001</v>
+      </c>
+      <c r="L13">
+        <v>0.26850000000000002</v>
+      </c>
+      <c r="M13">
+        <v>0.2457</v>
+      </c>
+      <c r="N13">
+        <v>0.23949999999999999</v>
+      </c>
+      <c r="O13">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="P13">
+        <v>11.7392</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L14">
+        <v>0.29220000000000002</v>
+      </c>
+      <c r="M14">
+        <v>0.2777</v>
+      </c>
+      <c r="N14">
+        <v>0.23830000000000001</v>
+      </c>
+      <c r="O14">
+        <v>0.1915</v>
+      </c>
+      <c r="P14">
+        <v>12.3285</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="G13">
-        <v>6.1999999999999998E-3</v>
-      </c>
-      <c r="H13">
-        <v>3.6600000000000001E-2</v>
-      </c>
-      <c r="I13">
-        <v>8.6300000000000002E-2</v>
-      </c>
-      <c r="J13">
-        <v>0.1154</v>
-      </c>
-      <c r="K13">
-        <v>0.14760000000000001</v>
-      </c>
-      <c r="L13">
-        <v>0.21379999999999999</v>
-      </c>
-      <c r="M13">
-        <v>0.1996</v>
-      </c>
-      <c r="N13">
-        <v>0.1356</v>
-      </c>
-      <c r="O13">
-        <v>5.8599999999999999E-2</v>
-      </c>
-      <c r="P13">
-        <v>10.8301</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>6.4999999999999997E-3</v>
-      </c>
-      <c r="R13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0.13270000000000001</v>
+      </c>
+      <c r="M15">
+        <v>0.2437</v>
+      </c>
+      <c r="N15">
+        <v>0.30320000000000003</v>
+      </c>
+      <c r="O15">
+        <v>0.32040000000000002</v>
+      </c>
+      <c r="P15">
+        <v>12.811299999999999</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="G14">
-        <v>5.1000000000000004E-3</v>
-      </c>
-      <c r="H14">
-        <v>2.8799999999999999E-2</v>
-      </c>
-      <c r="I14">
-        <v>6.7299999999999999E-2</v>
-      </c>
-      <c r="J14">
-        <v>8.7900000000000006E-2</v>
-      </c>
-      <c r="K14">
-        <v>0.11890000000000001</v>
-      </c>
-      <c r="L14">
-        <v>0.1988</v>
-      </c>
-      <c r="M14">
-        <v>0.20780000000000001</v>
-      </c>
-      <c r="N14">
-        <v>0.189</v>
-      </c>
-      <c r="O14">
-        <v>9.6100000000000005E-2</v>
-      </c>
-      <c r="P14">
-        <v>11.234999999999999</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="R14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>1E-4</v>
-      </c>
-      <c r="G15">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="H15">
-        <v>1.7299999999999999E-2</v>
-      </c>
-      <c r="I15">
-        <v>0.04</v>
-      </c>
-      <c r="J15">
-        <v>5.8200000000000002E-2</v>
-      </c>
-      <c r="K15">
-        <v>6.2300000000000001E-2</v>
-      </c>
-      <c r="L15">
-        <v>0.1172</v>
-      </c>
-      <c r="M15">
-        <v>0.18920000000000001</v>
-      </c>
-      <c r="N15">
-        <v>0.26050000000000001</v>
-      </c>
-      <c r="O15">
-        <v>0.25209999999999999</v>
-      </c>
-      <c r="P15">
-        <v>12.0825</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="R15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
       <c r="B16">
         <v>0</v>
       </c>
@@ -1333,25 +1333,25 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>5.5999999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>3.4299999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>7.4700000000000003E-2</v>
+        <v>0.1363</v>
       </c>
       <c r="M16">
-        <v>0.1111</v>
+        <v>0.2326</v>
       </c>
       <c r="N16">
-        <v>0.21829999999999999</v>
+        <v>0.219</v>
       </c>
       <c r="O16">
-        <v>0.55600000000000005</v>
+        <v>0.41210000000000002</v>
       </c>
       <c r="P16">
-        <v>13.170199999999999</v>
+        <v>12.9069</v>
       </c>
       <c r="Q16" s="1">
         <v>0</v>

</xml_diff>